<commit_message>
Edit of some test bank workbooks and get_data function to handle non-comma seperated entires/ entries that are strings
</commit_message>
<xml_diff>
--- a/test_spreadsheets/3-Cleaning Samples Template.xlsx
+++ b/test_spreadsheets/3-Cleaning Samples Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t xml:space="preserve">Sample Set:</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">delrin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test for typeerror exit</t>
   </si>
   <si>
     <t xml:space="preserve">nickel</t>
@@ -437,7 +440,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -657,8 +660,8 @@
       <c r="D17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="2" t="n">
-        <v>0.024</v>
+      <c r="E17" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>7.18</v>
@@ -672,7 +675,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>31</v>

</xml_diff>